<commit_message>
Add support for column formats
</commit_message>
<xml_diff>
--- a/src/Demo.xlsx
+++ b/src/Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="14820" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24921,7 +24921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -25316,8 +25316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N743"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25325,7 +25325,7 @@
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" style="19" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Add support for new-style formatting and the "match" field in Alfred 3.5
</commit_message>
<xml_diff>
--- a/src/Demo.xlsx
+++ b/src/Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="13660" windowHeight="14820" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6600,8 +6600,57 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7B7B7"/>
+          <bgColor rgb="FFB7B7B7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="Sheet1-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FF682894"/>

</xml_diff>